<commit_message>
xlsx machine id updated.
</commit_message>
<xml_diff>
--- a/send-data-to-mqtt-python/machines.xlsx
+++ b/send-data-to-mqtt-python/machines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SmartWeld\smartweld-mqtt-data-gen\send-data-to-mqtt-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBIW\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F806B66D-CABA-46B0-AA91-69E1BCB2C1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC0D2A1-2F16-4E8D-A74A-E30BC93E0418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="machines" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +172,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -515,9 +521,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -873,15 +880,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -942,6 +949,16 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>969247043362701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>865006042456120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>865006042456138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>